<commit_message>
big bug observed: work on the scrapping needs to be done
</commit_message>
<xml_diff>
--- a/data/results_international/scrap_out.xlsx
+++ b/data/results_international/scrap_out.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K100"/>
+  <dimension ref="A1:K148"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,22 +445,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>home_team</t>
+          <t>Team A</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>away_team</t>
+          <t>Team B</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>home_score</t>
+          <t>Score A</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>away_score</t>
+          <t>Score B</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -475,17 +475,17 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>city</t>
+          <t>City</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>country</t>
+          <t>Neut.</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Neut.</t>
+          <t>Country</t>
         </is>
       </c>
     </row>
@@ -527,13 +527,13 @@
           <t>Rome</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>Italy</t>
         </is>
-      </c>
-      <c r="K2" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -574,13 +574,13 @@
           <t>London</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>England</t>
         </is>
-      </c>
-      <c r="K3" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -621,13 +621,13 @@
           <t>Cardiff</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>Wales</t>
         </is>
-      </c>
-      <c r="K4" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -668,13 +668,13 @@
           <t>London</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>England</t>
         </is>
-      </c>
-      <c r="K5" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -715,13 +715,13 @@
           <t>Edinburgh</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" t="inlineStr">
         <is>
           <t>Scotland</t>
         </is>
-      </c>
-      <c r="K6" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -762,13 +762,13 @@
           <t>Dublin</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>Ireland</t>
         </is>
-      </c>
-      <c r="K7" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -809,13 +809,13 @@
           <t>Rome</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="inlineStr">
         <is>
           <t>Italy</t>
         </is>
-      </c>
-      <c r="K8" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -856,13 +856,13 @@
           <t>Cardiff</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>Wales</t>
         </is>
-      </c>
-      <c r="K9" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -903,13 +903,13 @@
           <t>Rome</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t>Italy</t>
         </is>
-      </c>
-      <c r="K10" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -950,13 +950,13 @@
           <t>London</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="inlineStr">
         <is>
           <t>England</t>
         </is>
-      </c>
-      <c r="K11" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -997,13 +997,13 @@
           <t>Edinburgh</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>Scotland</t>
         </is>
-      </c>
-      <c r="K12" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1044,13 +1044,13 @@
           <t>Edinburgh</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>Scotland</t>
         </is>
-      </c>
-      <c r="K13" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1091,13 +1091,13 @@
           <t>Dublin</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="inlineStr">
         <is>
           <t>Ireland</t>
         </is>
-      </c>
-      <c r="K14" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1138,13 +1138,13 @@
           <t>Saint-Denis</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="inlineStr">
         <is>
           <t>France</t>
         </is>
-      </c>
-      <c r="K15" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1185,13 +1185,13 @@
           <t>Saint-Denis</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="inlineStr">
         <is>
           <t>France</t>
         </is>
-      </c>
-      <c r="K16" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1232,13 +1232,13 @@
           <t>Dublin</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" t="inlineStr">
         <is>
           <t>Ireland</t>
         </is>
-      </c>
-      <c r="K17" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1279,13 +1279,13 @@
           <t>Edinburgh</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" t="inlineStr">
         <is>
           <t>Scotland</t>
         </is>
-      </c>
-      <c r="K18" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1326,13 +1326,13 @@
           <t>Saint-Denis</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="inlineStr">
         <is>
           <t>France</t>
         </is>
-      </c>
-      <c r="K19" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1373,13 +1373,13 @@
           <t>Cardiff</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="inlineStr">
         <is>
           <t>Wales</t>
         </is>
-      </c>
-      <c r="K20" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1420,13 +1420,13 @@
           <t>Saint-Denis</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr">
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" t="inlineStr">
         <is>
           <t>France</t>
         </is>
-      </c>
-      <c r="K21" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1467,13 +1467,13 @@
           <t>Rome</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr">
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" t="inlineStr">
         <is>
           <t>Italy</t>
         </is>
-      </c>
-      <c r="K22" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1514,13 +1514,13 @@
           <t>Edinburgh</t>
         </is>
       </c>
-      <c r="J23" t="inlineStr">
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" t="inlineStr">
         <is>
           <t>Scotland</t>
         </is>
-      </c>
-      <c r="K23" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1561,13 +1561,13 @@
           <t>London</t>
         </is>
       </c>
-      <c r="J24" t="inlineStr">
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" t="inlineStr">
         <is>
           <t>England</t>
         </is>
-      </c>
-      <c r="K24" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1608,13 +1608,13 @@
           <t>Dublin</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr">
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>Ireland</t>
         </is>
-      </c>
-      <c r="K25" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1655,13 +1655,13 @@
           <t>Cardiff</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
+      <c r="J26" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" t="inlineStr">
         <is>
           <t>Wales</t>
         </is>
-      </c>
-      <c r="K26" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1702,13 +1702,13 @@
           <t>Rome</t>
         </is>
       </c>
-      <c r="J27" t="inlineStr">
+      <c r="J27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K27" t="inlineStr">
         <is>
           <t>Italy</t>
         </is>
-      </c>
-      <c r="K27" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1749,13 +1749,13 @@
           <t>London</t>
         </is>
       </c>
-      <c r="J28" t="inlineStr">
+      <c r="J28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28" t="inlineStr">
         <is>
           <t>England</t>
         </is>
-      </c>
-      <c r="K28" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1796,13 +1796,13 @@
           <t>Cardiff</t>
         </is>
       </c>
-      <c r="J29" t="inlineStr">
+      <c r="J29" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" t="inlineStr">
         <is>
           <t>Wales</t>
         </is>
-      </c>
-      <c r="K29" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1843,13 +1843,13 @@
           <t>Dublin</t>
         </is>
       </c>
-      <c r="J30" t="inlineStr">
+      <c r="J30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K30" t="inlineStr">
         <is>
           <t>Ireland</t>
         </is>
-      </c>
-      <c r="K30" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1890,13 +1890,13 @@
           <t>Saint-Denis</t>
         </is>
       </c>
-      <c r="J31" t="inlineStr">
+      <c r="J31" t="b">
+        <v>0</v>
+      </c>
+      <c r="K31" t="inlineStr">
         <is>
           <t>France</t>
         </is>
-      </c>
-      <c r="K31" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1937,13 +1937,13 @@
           <t>Cardiff</t>
         </is>
       </c>
-      <c r="J32" t="inlineStr">
+      <c r="J32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" t="inlineStr">
         <is>
           <t>Wales</t>
         </is>
-      </c>
-      <c r="K32" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1984,13 +1984,13 @@
           <t>London</t>
         </is>
       </c>
-      <c r="J33" t="inlineStr">
+      <c r="J33" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" t="inlineStr">
         <is>
           <t>England</t>
         </is>
-      </c>
-      <c r="K33" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -2031,13 +2031,13 @@
           <t>Rome</t>
         </is>
       </c>
-      <c r="J34" t="inlineStr">
+      <c r="J34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" t="inlineStr">
         <is>
           <t>Italy</t>
         </is>
-      </c>
-      <c r="K34" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -2078,13 +2078,13 @@
           <t>Dublin</t>
         </is>
       </c>
-      <c r="J35" t="inlineStr">
+      <c r="J35" t="b">
+        <v>0</v>
+      </c>
+      <c r="K35" t="inlineStr">
         <is>
           <t>Ireland</t>
         </is>
-      </c>
-      <c r="K35" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -2125,13 +2125,13 @@
           <t>Edinburgh</t>
         </is>
       </c>
-      <c r="J36" t="inlineStr">
+      <c r="J36" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36" t="inlineStr">
         <is>
           <t>Scotland</t>
         </is>
-      </c>
-      <c r="K36" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -2172,13 +2172,13 @@
           <t>London</t>
         </is>
       </c>
-      <c r="J37" t="inlineStr">
+      <c r="J37" t="b">
+        <v>0</v>
+      </c>
+      <c r="K37" t="inlineStr">
         <is>
           <t>England</t>
         </is>
-      </c>
-      <c r="K37" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -2219,13 +2219,13 @@
           <t>Rome</t>
         </is>
       </c>
-      <c r="J38" t="inlineStr">
+      <c r="J38" t="b">
+        <v>0</v>
+      </c>
+      <c r="K38" t="inlineStr">
         <is>
           <t>Italy</t>
         </is>
-      </c>
-      <c r="K38" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -2266,13 +2266,13 @@
           <t>Cardiff</t>
         </is>
       </c>
-      <c r="J39" t="inlineStr">
+      <c r="J39" t="b">
+        <v>0</v>
+      </c>
+      <c r="K39" t="inlineStr">
         <is>
           <t>Wales</t>
         </is>
-      </c>
-      <c r="K39" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -2313,13 +2313,13 @@
           <t>Saint-Denis</t>
         </is>
       </c>
-      <c r="J40" t="inlineStr">
+      <c r="J40" t="b">
+        <v>0</v>
+      </c>
+      <c r="K40" t="inlineStr">
         <is>
           <t>France</t>
         </is>
-      </c>
-      <c r="K40" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -2360,13 +2360,13 @@
           <t>Rome</t>
         </is>
       </c>
-      <c r="J41" t="inlineStr">
+      <c r="J41" t="b">
+        <v>0</v>
+      </c>
+      <c r="K41" t="inlineStr">
         <is>
           <t>Italy</t>
         </is>
-      </c>
-      <c r="K41" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -2407,13 +2407,13 @@
           <t>London</t>
         </is>
       </c>
-      <c r="J42" t="inlineStr">
+      <c r="J42" t="b">
+        <v>0</v>
+      </c>
+      <c r="K42" t="inlineStr">
         <is>
           <t>England</t>
         </is>
-      </c>
-      <c r="K42" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -2454,13 +2454,13 @@
           <t>Edinburgh</t>
         </is>
       </c>
-      <c r="J43" t="inlineStr">
+      <c r="J43" t="b">
+        <v>0</v>
+      </c>
+      <c r="K43" t="inlineStr">
         <is>
           <t>Scotland</t>
         </is>
-      </c>
-      <c r="K43" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -2501,13 +2501,13 @@
           <t>Edinburgh</t>
         </is>
       </c>
-      <c r="J44" t="inlineStr">
+      <c r="J44" t="b">
+        <v>0</v>
+      </c>
+      <c r="K44" t="inlineStr">
         <is>
           <t>Scotland</t>
         </is>
-      </c>
-      <c r="K44" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -2548,13 +2548,13 @@
           <t>Saint-Denis</t>
         </is>
       </c>
-      <c r="J45" t="inlineStr">
+      <c r="J45" t="b">
+        <v>0</v>
+      </c>
+      <c r="K45" t="inlineStr">
         <is>
           <t>France</t>
         </is>
-      </c>
-      <c r="K45" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -2595,13 +2595,13 @@
           <t>Dublin</t>
         </is>
       </c>
-      <c r="J46" t="inlineStr">
+      <c r="J46" t="b">
+        <v>0</v>
+      </c>
+      <c r="K46" t="inlineStr">
         <is>
           <t>Ireland</t>
         </is>
-      </c>
-      <c r="K46" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -2642,13 +2642,13 @@
           <t>Auckland</t>
         </is>
       </c>
-      <c r="J47" t="inlineStr">
+      <c r="J47" t="b">
+        <v>0</v>
+      </c>
+      <c r="K47" t="inlineStr">
         <is>
           <t>New Zealand</t>
         </is>
-      </c>
-      <c r="K47" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -2689,13 +2689,13 @@
           <t>Port Elizabeth</t>
         </is>
       </c>
-      <c r="J48" t="inlineStr">
+      <c r="J48" t="b">
+        <v>0</v>
+      </c>
+      <c r="K48" t="inlineStr">
         <is>
           <t>South Africa</t>
         </is>
-      </c>
-      <c r="K48" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -2736,13 +2736,13 @@
           <t>Port Elizabeth</t>
         </is>
       </c>
-      <c r="J49" t="inlineStr">
+      <c r="J49" t="b">
+        <v>1</v>
+      </c>
+      <c r="K49" t="inlineStr">
         <is>
           <t>South Africa</t>
         </is>
-      </c>
-      <c r="K49" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -2783,13 +2783,13 @@
           <t>Perth</t>
         </is>
       </c>
-      <c r="J50" t="inlineStr">
+      <c r="J50" t="b">
+        <v>0</v>
+      </c>
+      <c r="K50" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
-      </c>
-      <c r="K50" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -2830,13 +2830,13 @@
           <t>Gold Coast</t>
         </is>
       </c>
-      <c r="J51" t="inlineStr">
+      <c r="J51" t="b">
+        <v>1</v>
+      </c>
+      <c r="K51" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
-      </c>
-      <c r="K51" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -2877,13 +2877,13 @@
           <t>Gold Coast [d]</t>
         </is>
       </c>
-      <c r="J52" t="inlineStr">
+      <c r="J52" t="b">
+        <v>1</v>
+      </c>
+      <c r="K52" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
-      </c>
-      <c r="K52" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -2924,13 +2924,13 @@
           <t>Brisbane</t>
         </is>
       </c>
-      <c r="J53" t="inlineStr">
+      <c r="J53" t="b">
+        <v>0</v>
+      </c>
+      <c r="K53" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
-      </c>
-      <c r="K53" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -2971,13 +2971,13 @@
           <t>Brisbane</t>
         </is>
       </c>
-      <c r="J54" t="inlineStr">
+      <c r="J54" t="b">
+        <v>1</v>
+      </c>
+      <c r="K54" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
-      </c>
-      <c r="K54" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -3018,13 +3018,13 @@
           <t>Townsville [e]</t>
         </is>
       </c>
-      <c r="J55" t="inlineStr">
+      <c r="J55" t="b">
+        <v>1</v>
+      </c>
+      <c r="K55" t="inlineStr">
         <is>
           <t>Ireland</t>
         </is>
-      </c>
-      <c r="K55" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -3065,13 +3065,13 @@
           <t>Townsville [f]</t>
         </is>
       </c>
-      <c r="J56" t="inlineStr">
+      <c r="J56" t="b">
+        <v>0</v>
+      </c>
+      <c r="K56" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
-      </c>
-      <c r="K56" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -3112,13 +3112,13 @@
           <t>Gold Coast [g]</t>
         </is>
       </c>
-      <c r="J57" t="inlineStr">
+      <c r="J57" t="b">
+        <v>1</v>
+      </c>
+      <c r="K57" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
-      </c>
-      <c r="K57" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -3159,13 +3159,13 @@
           <t>Gold Coast [h]</t>
         </is>
       </c>
-      <c r="J58" t="inlineStr">
+      <c r="J58" t="b">
+        <v>1</v>
+      </c>
+      <c r="K58" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
-      </c>
-      <c r="K58" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -3206,13 +3206,13 @@
           <t>Mbombela</t>
         </is>
       </c>
-      <c r="J59" t="inlineStr">
+      <c r="J59" t="b">
+        <v>0</v>
+      </c>
+      <c r="K59" t="inlineStr">
         <is>
           <t>South Africa</t>
         </is>
-      </c>
-      <c r="K59" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -3253,13 +3253,13 @@
           <t>Mendoza</t>
         </is>
       </c>
-      <c r="J60" t="inlineStr">
+      <c r="J60" t="b">
+        <v>0</v>
+      </c>
+      <c r="K60" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
-      </c>
-      <c r="K60" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -3300,13 +3300,13 @@
           <t>Johannesburg</t>
         </is>
       </c>
-      <c r="J61" t="inlineStr">
+      <c r="J61" t="b">
+        <v>0</v>
+      </c>
+      <c r="K61" t="inlineStr">
         <is>
           <t>South Africa</t>
         </is>
-      </c>
-      <c r="K61" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -3347,13 +3347,13 @@
           <t>San Juan</t>
         </is>
       </c>
-      <c r="J62" t="inlineStr">
+      <c r="J62" t="b">
+        <v>1</v>
+      </c>
+      <c r="K62" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
-      </c>
-      <c r="K62" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -3394,13 +3394,13 @@
           <t>Adelaide</t>
         </is>
       </c>
-      <c r="J63" t="inlineStr">
+      <c r="J63" t="b">
+        <v>0</v>
+      </c>
+      <c r="K63" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
-      </c>
-      <c r="K63" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -3441,13 +3441,13 @@
           <t>Christchurch</t>
         </is>
       </c>
-      <c r="J64" t="inlineStr">
+      <c r="J64" t="b">
+        <v>0</v>
+      </c>
+      <c r="K64" t="inlineStr">
         <is>
           <t>New Zealand</t>
         </is>
-      </c>
-      <c r="K64" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -3488,13 +3488,13 @@
           <t>Hamilton</t>
         </is>
       </c>
-      <c r="J65" t="inlineStr">
+      <c r="J65" t="b">
+        <v>1</v>
+      </c>
+      <c r="K65" t="inlineStr">
         <is>
           <t>Canada</t>
         </is>
-      </c>
-      <c r="K65" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -3535,13 +3535,13 @@
           <t>Sydney</t>
         </is>
       </c>
-      <c r="J66" t="inlineStr">
+      <c r="J66" t="b">
+        <v>0</v>
+      </c>
+      <c r="K66" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
-      </c>
-      <c r="K66" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -3582,13 +3582,13 @@
           <t>Melbourne</t>
         </is>
       </c>
-      <c r="J67" t="inlineStr">
+      <c r="J67" t="b">
+        <v>0</v>
+      </c>
+      <c r="K67" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
-      </c>
-      <c r="K67" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -3629,13 +3629,13 @@
           <t>Buenos Aires[a]</t>
         </is>
       </c>
-      <c r="J68" t="inlineStr">
+      <c r="J68" t="b">
+        <v>0</v>
+      </c>
+      <c r="K68" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
-      </c>
-      <c r="K68" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -3676,13 +3676,13 @@
           <t>Auckland</t>
         </is>
       </c>
-      <c r="J69" t="inlineStr">
+      <c r="J69" t="b">
+        <v>0</v>
+      </c>
+      <c r="K69" t="inlineStr">
         <is>
           <t>New Zealand</t>
         </is>
-      </c>
-      <c r="K69" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -3723,13 +3723,13 @@
           <t>Durban</t>
         </is>
       </c>
-      <c r="J70" t="inlineStr">
+      <c r="J70" t="b">
+        <v>0</v>
+      </c>
+      <c r="K70" t="inlineStr">
         <is>
           <t>South Africa</t>
         </is>
-      </c>
-      <c r="K70" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -3770,13 +3770,13 @@
           <t>Pretoria</t>
         </is>
       </c>
-      <c r="J71" t="inlineStr">
+      <c r="J71" t="b">
+        <v>0</v>
+      </c>
+      <c r="K71" t="inlineStr">
         <is>
           <t>South Africa</t>
         </is>
-      </c>
-      <c r="K71" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -3817,13 +3817,13 @@
           <t>Mendoza</t>
         </is>
       </c>
-      <c r="J72" t="inlineStr">
+      <c r="J72" t="b">
+        <v>0</v>
+      </c>
+      <c r="K72" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
-      </c>
-      <c r="K72" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -3864,13 +3864,13 @@
           <t>Auckland</t>
         </is>
       </c>
-      <c r="J73" t="inlineStr">
+      <c r="J73" t="b">
+        <v>0</v>
+      </c>
+      <c r="K73" t="inlineStr">
         <is>
           <t>New Zealand</t>
         </is>
-      </c>
-      <c r="K73" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -3911,13 +3911,13 @@
           <t>Sydney</t>
         </is>
       </c>
-      <c r="J74" t="inlineStr">
+      <c r="J74" t="b">
+        <v>0</v>
+      </c>
+      <c r="K74" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
-      </c>
-      <c r="K74" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -3958,13 +3958,13 @@
           <t>Melbourne</t>
         </is>
       </c>
-      <c r="J75" t="inlineStr">
+      <c r="J75" t="b">
+        <v>0</v>
+      </c>
+      <c r="K75" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
-      </c>
-      <c r="K75" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -4005,13 +4005,13 @@
           <t>Johannesburg</t>
         </is>
       </c>
-      <c r="J76" t="inlineStr">
+      <c r="J76" t="b">
+        <v>0</v>
+      </c>
+      <c r="K76" t="inlineStr">
         <is>
           <t>South Africa</t>
         </is>
-      </c>
-      <c r="K76" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -4052,13 +4052,13 @@
           <t>Suva</t>
         </is>
       </c>
-      <c r="J77" t="inlineStr">
+      <c r="J77" t="b">
+        <v>1</v>
+      </c>
+      <c r="K77" t="inlineStr">
         <is>
           <t>Fiji</t>
         </is>
-      </c>
-      <c r="K77" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -4099,13 +4099,13 @@
           <t>Suva</t>
         </is>
       </c>
-      <c r="J78" t="inlineStr">
+      <c r="J78" t="b">
+        <v>0</v>
+      </c>
+      <c r="K78" t="inlineStr">
         <is>
           <t>Fiji</t>
         </is>
-      </c>
-      <c r="K78" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -4146,13 +4146,13 @@
           <t>Lautoka</t>
         </is>
       </c>
-      <c r="J79" t="inlineStr">
+      <c r="J79" t="b">
+        <v>1</v>
+      </c>
+      <c r="K79" t="inlineStr">
         <is>
           <t>Fiji</t>
         </is>
-      </c>
-      <c r="K79" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -4193,13 +4193,13 @@
           <t>Lautoka</t>
         </is>
       </c>
-      <c r="J80" t="inlineStr">
+      <c r="J80" t="b">
+        <v>0</v>
+      </c>
+      <c r="K80" t="inlineStr">
         <is>
           <t>Fiji</t>
         </is>
-      </c>
-      <c r="K80" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -4240,13 +4240,13 @@
           <t>Lautoka</t>
         </is>
       </c>
-      <c r="J81" t="inlineStr">
+      <c r="J81" t="b">
+        <v>1</v>
+      </c>
+      <c r="K81" t="inlineStr">
         <is>
           <t>Fiji</t>
         </is>
-      </c>
-      <c r="K81" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -4287,13 +4287,13 @@
           <t>Lautoka</t>
         </is>
       </c>
-      <c r="J82" t="inlineStr">
+      <c r="J82" t="b">
+        <v>0</v>
+      </c>
+      <c r="K82" t="inlineStr">
         <is>
           <t>Fiji</t>
         </is>
-      </c>
-      <c r="K82" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -4334,13 +4334,13 @@
           <t>Lautoka</t>
         </is>
       </c>
-      <c r="J83" t="inlineStr">
+      <c r="J83" t="b">
+        <v>0</v>
+      </c>
+      <c r="K83" t="inlineStr">
         <is>
           <t>Fiji</t>
         </is>
-      </c>
-      <c r="K83" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -4381,13 +4381,13 @@
           <t>Sapporo</t>
         </is>
       </c>
-      <c r="J84" t="inlineStr">
+      <c r="J84" t="b">
+        <v>0</v>
+      </c>
+      <c r="K84" t="inlineStr">
         <is>
           <t>Japan</t>
         </is>
-      </c>
-      <c r="K84" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -4428,13 +4428,13 @@
           <t>Apia</t>
         </is>
       </c>
-      <c r="J85" t="inlineStr">
+      <c r="J85" t="b">
+        <v>0</v>
+      </c>
+      <c r="K85" t="inlineStr">
         <is>
           <t>Samoa</t>
         </is>
-      </c>
-      <c r="K85" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -4475,13 +4475,13 @@
           <t>Higashiōsaka</t>
         </is>
       </c>
-      <c r="J86" t="inlineStr">
+      <c r="J86" t="b">
+        <v>0</v>
+      </c>
+      <c r="K86" t="inlineStr">
         <is>
           <t>Japan</t>
         </is>
-      </c>
-      <c r="K86" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -4522,13 +4522,13 @@
           <t>Apia</t>
         </is>
       </c>
-      <c r="J87" t="inlineStr">
+      <c r="J87" t="b">
+        <v>0</v>
+      </c>
+      <c r="K87" t="inlineStr">
         <is>
           <t>Samoa</t>
         </is>
-      </c>
-      <c r="K87" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -4569,13 +4569,13 @@
           <t>Tokyo</t>
         </is>
       </c>
-      <c r="J88" t="inlineStr">
+      <c r="J88" t="b">
+        <v>0</v>
+      </c>
+      <c r="K88" t="inlineStr">
         <is>
           <t>Japan</t>
         </is>
-      </c>
-      <c r="K88" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -4616,13 +4616,13 @@
           <t>Lahore</t>
         </is>
       </c>
-      <c r="J89" t="inlineStr">
+      <c r="J89" t="b">
+        <v>0</v>
+      </c>
+      <c r="K89" t="inlineStr">
         <is>
           <t>Pakistan</t>
         </is>
-      </c>
-      <c r="K89" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -4663,13 +4663,13 @@
           <t>Lahore</t>
         </is>
       </c>
-      <c r="J90" t="inlineStr">
+      <c r="J90" t="b">
+        <v>0</v>
+      </c>
+      <c r="K90" t="inlineStr">
         <is>
           <t>Pakistan</t>
         </is>
-      </c>
-      <c r="K90" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -4710,13 +4710,13 @@
           <t>Bishkek</t>
         </is>
       </c>
-      <c r="J91" t="inlineStr">
+      <c r="J91" t="b">
+        <v>1</v>
+      </c>
+      <c r="K91" t="inlineStr">
         <is>
           <t>Kyrgyzstan</t>
         </is>
-      </c>
-      <c r="K91" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -4757,13 +4757,13 @@
           <t>Bishkek</t>
         </is>
       </c>
-      <c r="J92" t="inlineStr">
+      <c r="J92" t="b">
+        <v>0</v>
+      </c>
+      <c r="K92" t="inlineStr">
         <is>
           <t>Kyrgyzstan</t>
         </is>
-      </c>
-      <c r="K92" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -4804,13 +4804,13 @@
           <t>Bishkek</t>
         </is>
       </c>
-      <c r="J93" t="inlineStr">
+      <c r="J93" t="b">
+        <v>0</v>
+      </c>
+      <c r="K93" t="inlineStr">
         <is>
           <t>Kyrgyzstan</t>
         </is>
-      </c>
-      <c r="K93" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -4851,13 +4851,13 @@
           <t>Bishkek</t>
         </is>
       </c>
-      <c r="J94" t="inlineStr">
+      <c r="J94" t="b">
+        <v>1</v>
+      </c>
+      <c r="K94" t="inlineStr">
         <is>
           <t>Kyrgyzstan</t>
         </is>
-      </c>
-      <c r="K94" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="95">
@@ -4898,13 +4898,13 @@
           <t>Kolkata</t>
         </is>
       </c>
-      <c r="J95" t="inlineStr">
+      <c r="J95" t="b">
+        <v>0</v>
+      </c>
+      <c r="K95" t="inlineStr">
         <is>
           <t>India</t>
         </is>
-      </c>
-      <c r="K95" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -4945,13 +4945,13 @@
           <t>Kolkata</t>
         </is>
       </c>
-      <c r="J96" t="inlineStr">
+      <c r="J96" t="b">
+        <v>1</v>
+      </c>
+      <c r="K96" t="inlineStr">
         <is>
           <t>India</t>
         </is>
-      </c>
-      <c r="K96" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="97">
@@ -4992,13 +4992,13 @@
           <t>Kolkata</t>
         </is>
       </c>
-      <c r="J97" t="inlineStr">
+      <c r="J97" t="b">
+        <v>0</v>
+      </c>
+      <c r="K97" t="inlineStr">
         <is>
           <t>India</t>
         </is>
-      </c>
-      <c r="K97" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -5039,13 +5039,13 @@
           <t>Kuala Lumpur</t>
         </is>
       </c>
-      <c r="J98" t="inlineStr">
+      <c r="J98" t="b">
+        <v>0</v>
+      </c>
+      <c r="K98" t="inlineStr">
         <is>
           <t>Malaysia</t>
         </is>
-      </c>
-      <c r="K98" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -5086,13 +5086,13 @@
           <t>Hong Kong</t>
         </is>
       </c>
-      <c r="J99" t="inlineStr">
+      <c r="J99" t="b">
+        <v>1</v>
+      </c>
+      <c r="K99" t="inlineStr">
         <is>
           <t>China</t>
         </is>
-      </c>
-      <c r="K99" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="100">
@@ -5133,13 +5133,2269 @@
           <t>Hong Kong</t>
         </is>
       </c>
-      <c r="J100" t="inlineStr">
+      <c r="J100" t="b">
+        <v>1</v>
+      </c>
+      <c r="K100" t="inlineStr">
         <is>
           <t>China</t>
         </is>
       </c>
-      <c r="K100" t="b">
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" s="2" t="n">
+        <v>45227</v>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>South Africa</t>
+        </is>
+      </c>
+      <c r="E101" t="n">
+        <v>11</v>
+      </c>
+      <c r="F101" t="n">
+        <v>12</v>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J101" t="b">
+        <v>0</v>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" s="2" t="n">
+        <v>45226</v>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+      <c r="E102" t="n">
+        <v>23</v>
+      </c>
+      <c r="F102" t="n">
+        <v>26</v>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J102" t="b">
         <v>1</v>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" s="2" t="n">
+        <v>45220</v>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>South Africa</t>
+        </is>
+      </c>
+      <c r="E103" t="n">
+        <v>15</v>
+      </c>
+      <c r="F103" t="n">
+        <v>16</v>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J103" t="b">
+        <v>1</v>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" s="2" t="n">
+        <v>45219</v>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="E104" t="n">
+        <v>44</v>
+      </c>
+      <c r="F104" t="n">
+        <v>6</v>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J104" t="b">
+        <v>0</v>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" s="2" t="n">
+        <v>45214</v>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>South Africa</t>
+        </is>
+      </c>
+      <c r="E105" t="n">
+        <v>28</v>
+      </c>
+      <c r="F105" t="n">
+        <v>29</v>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J105" t="b">
+        <v>1</v>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" s="2" t="n">
+        <v>45214</v>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Fiji</t>
+        </is>
+      </c>
+      <c r="E106" t="n">
+        <v>30</v>
+      </c>
+      <c r="F106" t="n">
+        <v>24</v>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J106" t="b">
+        <v>1</v>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" s="2" t="n">
+        <v>45213</v>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="E107" t="n">
+        <v>28</v>
+      </c>
+      <c r="F107" t="n">
+        <v>24</v>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J107" t="b">
+        <v>0</v>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" s="2" t="n">
+        <v>45213</v>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Wales</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="E108" t="n">
+        <v>17</v>
+      </c>
+      <c r="F108" t="n">
+        <v>29</v>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J108" t="b">
+        <v>1</v>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" s="2" t="n">
+        <v>45207</v>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Fiji</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="E109" t="n">
+        <v>23</v>
+      </c>
+      <c r="F109" t="n">
+        <v>24</v>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J109" t="b">
+        <v>1</v>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" s="2" t="n">
+        <v>45207</v>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Tonga</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Romania</t>
+        </is>
+      </c>
+      <c r="E110" t="n">
+        <v>45</v>
+      </c>
+      <c r="F110" t="n">
+        <v>24</v>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J110" t="b">
+        <v>1</v>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" s="2" t="n">
+        <v>45207</v>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Japan</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="E111" t="n">
+        <v>27</v>
+      </c>
+      <c r="F111" t="n">
+        <v>39</v>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J111" t="b">
+        <v>1</v>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" s="2" t="n">
+        <v>45206</v>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Scotland</t>
+        </is>
+      </c>
+      <c r="E112" t="n">
+        <v>36</v>
+      </c>
+      <c r="F112" t="n">
+        <v>14</v>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J112" t="b">
+        <v>1</v>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" s="2" t="n">
+        <v>45206</v>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Samoa</t>
+        </is>
+      </c>
+      <c r="E113" t="n">
+        <v>18</v>
+      </c>
+      <c r="F113" t="n">
+        <v>17</v>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J113" t="b">
+        <v>1</v>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" s="2" t="n">
+        <v>45206</v>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Wales</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="E114" t="n">
+        <v>43</v>
+      </c>
+      <c r="F114" t="n">
+        <v>19</v>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J114" t="b">
+        <v>1</v>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" s="2" t="n">
+        <v>45205</v>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="E115" t="n">
+        <v>60</v>
+      </c>
+      <c r="F115" t="n">
+        <v>7</v>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J115" t="b">
+        <v>1</v>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" s="2" t="n">
+        <v>45204</v>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Uruguay</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>73</v>
+      </c>
+      <c r="F116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J116" t="b">
+        <v>0</v>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" s="2" t="n">
+        <v>45200</v>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>South Africa</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Tonga</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>49</v>
+      </c>
+      <c r="F117" t="n">
+        <v>18</v>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J117" t="b">
+        <v>1</v>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" s="2" t="n">
+        <v>45200</v>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>34</v>
+      </c>
+      <c r="F118" t="n">
+        <v>14</v>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J118" t="b">
+        <v>1</v>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" s="2" t="n">
+        <v>45199</v>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Scotland</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Romania</t>
+        </is>
+      </c>
+      <c r="E119" t="n">
+        <v>84</v>
+      </c>
+      <c r="F119" t="n">
+        <v>0</v>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J119" t="b">
+        <v>1</v>
+      </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" s="2" t="n">
+        <v>45199</v>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Fiji</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="E120" t="n">
+        <v>17</v>
+      </c>
+      <c r="F120" t="n">
+        <v>12</v>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J120" t="b">
+        <v>1</v>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" s="2" t="n">
+        <v>45199</v>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Chile</t>
+        </is>
+      </c>
+      <c r="E121" t="n">
+        <v>59</v>
+      </c>
+      <c r="F121" t="n">
+        <v>5</v>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J121" t="b">
+        <v>1</v>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" s="2" t="n">
+        <v>45198</v>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="E122" t="n">
+        <v>96</v>
+      </c>
+      <c r="F122" t="n">
+        <v>17</v>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J122" t="b">
+        <v>0</v>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" s="2" t="n">
+        <v>45197</v>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Japan</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Samoa</t>
+        </is>
+      </c>
+      <c r="E123" t="n">
+        <v>28</v>
+      </c>
+      <c r="F123" t="n">
+        <v>22</v>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J123" t="b">
+        <v>1</v>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" s="2" t="n">
+        <v>45196</v>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Uruguay</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Namibia</t>
+        </is>
+      </c>
+      <c r="E124" t="n">
+        <v>36</v>
+      </c>
+      <c r="F124" t="n">
+        <v>26</v>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J124" t="b">
+        <v>1</v>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" s="2" t="n">
+        <v>45193</v>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Wales</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="E125" t="n">
+        <v>40</v>
+      </c>
+      <c r="F125" t="n">
+        <v>6</v>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J125" t="b">
+        <v>1</v>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" s="2" t="n">
+        <v>45193</v>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Scotland</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Tonga</t>
+        </is>
+      </c>
+      <c r="E126" t="n">
+        <v>45</v>
+      </c>
+      <c r="F126" t="n">
+        <v>17</v>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J126" t="b">
+        <v>1</v>
+      </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" s="2" t="n">
+        <v>45192</v>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>South Africa</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="E127" t="n">
+        <v>8</v>
+      </c>
+      <c r="F127" t="n">
+        <v>13</v>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J127" t="b">
+        <v>1</v>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" s="2" t="n">
+        <v>45192</v>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Chile</t>
+        </is>
+      </c>
+      <c r="E128" t="n">
+        <v>71</v>
+      </c>
+      <c r="F128" t="n">
+        <v>0</v>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J128" t="b">
+        <v>1</v>
+      </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" s="2" t="n">
+        <v>45192</v>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="E129" t="n">
+        <v>18</v>
+      </c>
+      <c r="F129" t="n">
+        <v>18</v>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J129" t="b">
+        <v>1</v>
+      </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" s="2" t="n">
+        <v>45191</v>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Samoa</t>
+        </is>
+      </c>
+      <c r="E130" t="n">
+        <v>19</v>
+      </c>
+      <c r="F130" t="n">
+        <v>10</v>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J130" t="b">
+        <v>1</v>
+      </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" s="2" t="n">
+        <v>45190</v>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Namibia</t>
+        </is>
+      </c>
+      <c r="E131" t="n">
+        <v>96</v>
+      </c>
+      <c r="F131" t="n">
+        <v>0</v>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J131" t="b">
+        <v>1</v>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" s="2" t="n">
+        <v>45189</v>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Uruguay</t>
+        </is>
+      </c>
+      <c r="E132" t="n">
+        <v>38</v>
+      </c>
+      <c r="F132" t="n">
+        <v>17</v>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J132" t="b">
+        <v>1</v>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" s="2" t="n">
+        <v>45186</v>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Japan</t>
+        </is>
+      </c>
+      <c r="E133" t="n">
+        <v>34</v>
+      </c>
+      <c r="F133" t="n">
+        <v>12</v>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J133" t="b">
+        <v>1</v>
+      </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" s="2" t="n">
+        <v>45186</v>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Fiji</t>
+        </is>
+      </c>
+      <c r="E134" t="n">
+        <v>15</v>
+      </c>
+      <c r="F134" t="n">
+        <v>22</v>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J134" t="b">
+        <v>1</v>
+      </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" s="2" t="n">
+        <v>45186</v>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>South Africa</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Romania</t>
+        </is>
+      </c>
+      <c r="E135" t="n">
+        <v>76</v>
+      </c>
+      <c r="F135" t="n">
+        <v>0</v>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J135" t="b">
+        <v>1</v>
+      </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" s="2" t="n">
+        <v>45185</v>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Tonga</t>
+        </is>
+      </c>
+      <c r="E136" t="n">
+        <v>59</v>
+      </c>
+      <c r="F136" t="n">
+        <v>16</v>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J136" t="b">
+        <v>1</v>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" s="2" t="n">
+        <v>45185</v>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Wales</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="E137" t="n">
+        <v>28</v>
+      </c>
+      <c r="F137" t="n">
+        <v>8</v>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J137" t="b">
+        <v>1</v>
+      </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" s="2" t="n">
+        <v>45185</v>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Samoa</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Chile</t>
+        </is>
+      </c>
+      <c r="E138" t="n">
+        <v>43</v>
+      </c>
+      <c r="F138" t="n">
+        <v>10</v>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J138" t="b">
+        <v>1</v>
+      </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" s="2" t="n">
+        <v>45184</v>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Namibia</t>
+        </is>
+      </c>
+      <c r="E139" t="n">
+        <v>71</v>
+      </c>
+      <c r="F139" t="n">
+        <v>3</v>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J139" t="b">
+        <v>0</v>
+      </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" s="2" t="n">
+        <v>45183</v>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Uruguay</t>
+        </is>
+      </c>
+      <c r="E140" t="n">
+        <v>27</v>
+      </c>
+      <c r="F140" t="n">
+        <v>12</v>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J140" t="b">
+        <v>1</v>
+      </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" s="2" t="n">
+        <v>45179</v>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Wales</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Fiji</t>
+        </is>
+      </c>
+      <c r="E141" t="n">
+        <v>32</v>
+      </c>
+      <c r="F141" t="n">
+        <v>26</v>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J141" t="b">
+        <v>1</v>
+      </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" s="2" t="n">
+        <v>45179</v>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>South Africa</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Scotland</t>
+        </is>
+      </c>
+      <c r="E142" t="n">
+        <v>18</v>
+      </c>
+      <c r="F142" t="n">
+        <v>3</v>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J142" t="b">
+        <v>1</v>
+      </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" s="2" t="n">
+        <v>45179</v>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Japan</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Chile</t>
+        </is>
+      </c>
+      <c r="E143" t="n">
+        <v>42</v>
+      </c>
+      <c r="F143" t="n">
+        <v>12</v>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J143" t="b">
+        <v>1</v>
+      </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" s="2" t="n">
+        <v>45178</v>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="E144" t="n">
+        <v>27</v>
+      </c>
+      <c r="F144" t="n">
+        <v>10</v>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J144" t="b">
+        <v>1</v>
+      </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" s="2" t="n">
+        <v>45178</v>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>35</v>
+      </c>
+      <c r="F145" t="n">
+        <v>15</v>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J145" t="b">
+        <v>1</v>
+      </c>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" s="2" t="n">
+        <v>45178</v>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Romania</t>
+        </is>
+      </c>
+      <c r="E146" t="n">
+        <v>82</v>
+      </c>
+      <c r="F146" t="n">
+        <v>8</v>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J146" t="b">
+        <v>1</v>
+      </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" s="2" t="n">
+        <v>45178</v>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Namibia</t>
+        </is>
+      </c>
+      <c r="E147" t="n">
+        <v>52</v>
+      </c>
+      <c r="F147" t="n">
+        <v>8</v>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J147" t="b">
+        <v>1</v>
+      </c>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" s="2" t="n">
+        <v>45177</v>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="E148" t="n">
+        <v>13</v>
+      </c>
+      <c r="F148" t="n">
+        <v>27</v>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>Auckland</t>
+        </is>
+      </c>
+      <c r="J148" t="b">
+        <v>0</v>
+      </c>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>New Zealand</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>